<commit_message>
minor change to product backlog
</commit_message>
<xml_diff>
--- a/Documentation/Product_Backlog.xlsx
+++ b/Documentation/Product_Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="8250"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="19440" windowHeight="8250"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -462,24 +462,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -490,15 +499,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -831,8 +831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -855,26 +855,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="I2" s="24" t="s">
+      <c r="I2" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="26"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="28"/>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="29"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -900,14 +900,14 @@
       </c>
       <c r="J3" s="8"/>
       <c r="K3" s="3"/>
-      <c r="L3" s="18" t="s">
+      <c r="L3" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="18"/>
-      <c r="N3" s="18"/>
-      <c r="O3" s="18"/>
-      <c r="P3" s="18"/>
-      <c r="Q3" s="19"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="25"/>
+      <c r="P3" s="25"/>
+      <c r="Q3" s="26"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -926,21 +926,21 @@
         <v>12</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>14</v>
       </c>
       <c r="J4" s="8"/>
       <c r="K4" s="4"/>
-      <c r="L4" s="20" t="s">
+      <c r="L4" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="M4" s="20"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="20"/>
-      <c r="P4" s="20"/>
-      <c r="Q4" s="21"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="19"/>
+      <c r="Q4" s="20"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -1034,17 +1034,17 @@
       <c r="F8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I8" s="24" t="s">
+      <c r="I8" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
-      <c r="L8" s="25"/>
-      <c r="M8" s="25"/>
-      <c r="N8" s="25"/>
-      <c r="O8" s="25"/>
-      <c r="P8" s="25"/>
-      <c r="Q8" s="26"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="29"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -1075,12 +1075,12 @@
       <c r="L9" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="M9" s="28" t="s">
+      <c r="M9" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="N9" s="18"/>
-      <c r="O9" s="18"/>
-      <c r="P9" s="19"/>
+      <c r="N9" s="25"/>
+      <c r="O9" s="25"/>
+      <c r="P9" s="26"/>
       <c r="Q9" s="11" t="s">
         <v>3</v>
       </c>
@@ -1113,10 +1113,10 @@
       <c r="L10" s="14">
         <v>40819</v>
       </c>
-      <c r="M10" s="29"/>
-      <c r="N10" s="20"/>
-      <c r="O10" s="20"/>
-      <c r="P10" s="21"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="20"/>
       <c r="Q10" s="12"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -1147,10 +1147,10 @@
       <c r="L11" s="14">
         <v>40826</v>
       </c>
-      <c r="M11" s="29"/>
-      <c r="N11" s="20"/>
-      <c r="O11" s="20"/>
-      <c r="P11" s="21"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="20"/>
       <c r="Q11" s="12"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -1181,10 +1181,10 @@
       <c r="L12" s="14">
         <v>40833</v>
       </c>
-      <c r="M12" s="29"/>
-      <c r="N12" s="20"/>
-      <c r="O12" s="20"/>
-      <c r="P12" s="21"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="19"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="20"/>
       <c r="Q12" s="12"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -1197,10 +1197,10 @@
       <c r="L13" s="14">
         <v>40840</v>
       </c>
-      <c r="M13" s="29"/>
-      <c r="N13" s="20"/>
-      <c r="O13" s="20"/>
-      <c r="P13" s="21"/>
+      <c r="M13" s="18"/>
+      <c r="N13" s="19"/>
+      <c r="O13" s="19"/>
+      <c r="P13" s="20"/>
       <c r="Q13" s="12"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -1213,10 +1213,10 @@
       <c r="L14" s="14">
         <v>40847</v>
       </c>
-      <c r="M14" s="29"/>
-      <c r="N14" s="20"/>
-      <c r="O14" s="20"/>
-      <c r="P14" s="21"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="19"/>
+      <c r="O14" s="19"/>
+      <c r="P14" s="20"/>
       <c r="Q14" s="12"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -1229,10 +1229,10 @@
       <c r="L15" s="14">
         <v>40854</v>
       </c>
-      <c r="M15" s="29"/>
-      <c r="N15" s="20"/>
-      <c r="O15" s="20"/>
-      <c r="P15" s="21"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="19"/>
+      <c r="O15" s="19"/>
+      <c r="P15" s="20"/>
       <c r="Q15" s="12"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
@@ -1245,10 +1245,10 @@
       <c r="L16" s="14">
         <v>40861</v>
       </c>
-      <c r="M16" s="29"/>
-      <c r="N16" s="20"/>
-      <c r="O16" s="20"/>
-      <c r="P16" s="21"/>
+      <c r="M16" s="18"/>
+      <c r="N16" s="19"/>
+      <c r="O16" s="19"/>
+      <c r="P16" s="20"/>
       <c r="Q16" s="12"/>
     </row>
     <row r="17" spans="9:17" x14ac:dyDescent="0.25">
@@ -1261,10 +1261,10 @@
       <c r="L17" s="14">
         <v>40868</v>
       </c>
-      <c r="M17" s="29"/>
-      <c r="N17" s="20"/>
-      <c r="O17" s="20"/>
-      <c r="P17" s="21"/>
+      <c r="M17" s="18"/>
+      <c r="N17" s="19"/>
+      <c r="O17" s="19"/>
+      <c r="P17" s="20"/>
       <c r="Q17" s="12"/>
     </row>
     <row r="18" spans="9:17" x14ac:dyDescent="0.25">
@@ -1277,10 +1277,10 @@
       <c r="L18" s="14">
         <v>40875</v>
       </c>
-      <c r="M18" s="29"/>
-      <c r="N18" s="20"/>
-      <c r="O18" s="20"/>
-      <c r="P18" s="21"/>
+      <c r="M18" s="18"/>
+      <c r="N18" s="19"/>
+      <c r="O18" s="19"/>
+      <c r="P18" s="20"/>
       <c r="Q18" s="12"/>
     </row>
     <row r="19" spans="9:17" x14ac:dyDescent="0.25">
@@ -1293,10 +1293,10 @@
       <c r="L19" s="14">
         <v>40882</v>
       </c>
-      <c r="M19" s="29"/>
-      <c r="N19" s="20"/>
-      <c r="O19" s="20"/>
-      <c r="P19" s="21"/>
+      <c r="M19" s="18"/>
+      <c r="N19" s="19"/>
+      <c r="O19" s="19"/>
+      <c r="P19" s="20"/>
       <c r="Q19" s="12"/>
     </row>
     <row r="20" spans="9:17" x14ac:dyDescent="0.25">
@@ -1309,10 +1309,10 @@
       <c r="L20" s="14">
         <v>40889</v>
       </c>
-      <c r="M20" s="29"/>
-      <c r="N20" s="20"/>
-      <c r="O20" s="20"/>
-      <c r="P20" s="21"/>
+      <c r="M20" s="18"/>
+      <c r="N20" s="19"/>
+      <c r="O20" s="19"/>
+      <c r="P20" s="20"/>
       <c r="Q20" s="16" t="s">
         <v>49</v>
       </c>
@@ -1327,7 +1327,7 @@
       <c r="L21" s="15">
         <v>40896</v>
       </c>
-      <c r="M21" s="30"/>
+      <c r="M21" s="21"/>
       <c r="N21" s="22"/>
       <c r="O21" s="22"/>
       <c r="P21" s="23"/>
@@ -1337,6 +1337,17 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="L3:Q3"/>
+    <mergeCell ref="L4:Q4"/>
+    <mergeCell ref="L5:Q5"/>
+    <mergeCell ref="I8:Q8"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="I2:Q2"/>
+    <mergeCell ref="M9:P9"/>
+    <mergeCell ref="M10:P10"/>
+    <mergeCell ref="M11:P11"/>
+    <mergeCell ref="M12:P12"/>
+    <mergeCell ref="M13:P13"/>
     <mergeCell ref="M20:P20"/>
     <mergeCell ref="M21:P21"/>
     <mergeCell ref="M14:P14"/>
@@ -1345,17 +1356,6 @@
     <mergeCell ref="M17:P17"/>
     <mergeCell ref="M18:P18"/>
     <mergeCell ref="M19:P19"/>
-    <mergeCell ref="M9:P9"/>
-    <mergeCell ref="M10:P10"/>
-    <mergeCell ref="M11:P11"/>
-    <mergeCell ref="M12:P12"/>
-    <mergeCell ref="M13:P13"/>
-    <mergeCell ref="L3:Q3"/>
-    <mergeCell ref="L4:Q4"/>
-    <mergeCell ref="L5:Q5"/>
-    <mergeCell ref="I8:Q8"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="I2:Q2"/>
   </mergeCells>
   <conditionalFormatting sqref="F4:F12">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="NOT STARTED">

</xml_diff>

<commit_message>
Update to Product Backlog
</commit_message>
<xml_diff>
--- a/Documentation/Product_Backlog.xlsx
+++ b/Documentation/Product_Backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="105">
   <si>
     <t>Product Backlog</t>
   </si>
@@ -319,6 +319,18 @@
   </si>
   <si>
     <t>Level Manager</t>
+  </si>
+  <si>
+    <t>Game Treatment 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comic Book Style Storyboard </t>
+  </si>
+  <si>
+    <t>Provice Concept Art Backlog</t>
+  </si>
+  <si>
+    <t>Art 8</t>
   </si>
 </sst>
 </file>
@@ -594,24 +606,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -622,64 +643,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF2FF146"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF2FF146"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -1003,10 +973,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q34"/>
+  <dimension ref="A1:Q36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1029,26 +999,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="I2" s="24" t="s">
+      <c r="I2" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="26"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="28"/>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="29"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1074,14 +1045,14 @@
       </c>
       <c r="J3" s="8"/>
       <c r="K3" s="3"/>
-      <c r="L3" s="18" t="s">
+      <c r="L3" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="18"/>
-      <c r="N3" s="18"/>
-      <c r="O3" s="18"/>
-      <c r="P3" s="18"/>
-      <c r="Q3" s="19"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="25"/>
+      <c r="P3" s="25"/>
+      <c r="Q3" s="26"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -1107,14 +1078,14 @@
       </c>
       <c r="J4" s="8"/>
       <c r="K4" s="4"/>
-      <c r="L4" s="20" t="s">
+      <c r="L4" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="M4" s="20"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="20"/>
-      <c r="P4" s="20"/>
-      <c r="Q4" s="21"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="19"/>
+      <c r="Q4" s="20"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -1208,17 +1179,17 @@
       <c r="F8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I8" s="24" t="s">
+      <c r="I8" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
-      <c r="L8" s="25"/>
-      <c r="M8" s="25"/>
-      <c r="N8" s="25"/>
-      <c r="O8" s="25"/>
-      <c r="P8" s="25"/>
-      <c r="Q8" s="26"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="29"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -1249,12 +1220,12 @@
       <c r="L9" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="M9" s="28" t="s">
+      <c r="M9" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="N9" s="18"/>
-      <c r="O9" s="18"/>
-      <c r="P9" s="19"/>
+      <c r="N9" s="25"/>
+      <c r="O9" s="25"/>
+      <c r="P9" s="26"/>
       <c r="Q9" s="11" t="s">
         <v>3</v>
       </c>
@@ -1287,10 +1258,10 @@
       <c r="L10" s="14">
         <v>40819</v>
       </c>
-      <c r="M10" s="29"/>
-      <c r="N10" s="20"/>
-      <c r="O10" s="20"/>
-      <c r="P10" s="21"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="20"/>
       <c r="Q10" s="12"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -1321,10 +1292,10 @@
       <c r="L11" s="14">
         <v>40826</v>
       </c>
-      <c r="M11" s="29"/>
-      <c r="N11" s="20"/>
-      <c r="O11" s="20"/>
-      <c r="P11" s="21"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="20"/>
       <c r="Q11" s="12"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -1355,10 +1326,10 @@
       <c r="L12" s="14">
         <v>40833</v>
       </c>
-      <c r="M12" s="29"/>
-      <c r="N12" s="20"/>
-      <c r="O12" s="20"/>
-      <c r="P12" s="21"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="19"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="20"/>
       <c r="Q12" s="12"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -1389,10 +1360,10 @@
       <c r="L13" s="14">
         <v>40840</v>
       </c>
-      <c r="M13" s="29"/>
-      <c r="N13" s="20"/>
-      <c r="O13" s="20"/>
-      <c r="P13" s="21"/>
+      <c r="M13" s="18"/>
+      <c r="N13" s="19"/>
+      <c r="O13" s="19"/>
+      <c r="P13" s="20"/>
       <c r="Q13" s="12"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -1423,10 +1394,10 @@
       <c r="L14" s="14">
         <v>40847</v>
       </c>
-      <c r="M14" s="29"/>
-      <c r="N14" s="20"/>
-      <c r="O14" s="20"/>
-      <c r="P14" s="21"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="19"/>
+      <c r="O14" s="19"/>
+      <c r="P14" s="20"/>
       <c r="Q14" s="12"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -1457,10 +1428,10 @@
       <c r="L15" s="14">
         <v>40854</v>
       </c>
-      <c r="M15" s="29"/>
-      <c r="N15" s="20"/>
-      <c r="O15" s="20"/>
-      <c r="P15" s="21"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="19"/>
+      <c r="O15" s="19"/>
+      <c r="P15" s="20"/>
       <c r="Q15" s="12"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
@@ -1491,10 +1462,10 @@
       <c r="L16" s="14">
         <v>40861</v>
       </c>
-      <c r="M16" s="29"/>
-      <c r="N16" s="20"/>
-      <c r="O16" s="20"/>
-      <c r="P16" s="21"/>
+      <c r="M16" s="18"/>
+      <c r="N16" s="19"/>
+      <c r="O16" s="19"/>
+      <c r="P16" s="20"/>
       <c r="Q16" s="12"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
@@ -1525,10 +1496,10 @@
       <c r="L17" s="14">
         <v>40868</v>
       </c>
-      <c r="M17" s="29"/>
-      <c r="N17" s="20"/>
-      <c r="O17" s="20"/>
-      <c r="P17" s="21"/>
+      <c r="M17" s="18"/>
+      <c r="N17" s="19"/>
+      <c r="O17" s="19"/>
+      <c r="P17" s="20"/>
       <c r="Q17" s="12"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
@@ -1559,10 +1530,10 @@
       <c r="L18" s="14">
         <v>40875</v>
       </c>
-      <c r="M18" s="29"/>
-      <c r="N18" s="20"/>
-      <c r="O18" s="20"/>
-      <c r="P18" s="21"/>
+      <c r="M18" s="18"/>
+      <c r="N18" s="19"/>
+      <c r="O18" s="19"/>
+      <c r="P18" s="20"/>
       <c r="Q18" s="12"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
@@ -1593,10 +1564,10 @@
       <c r="L19" s="14">
         <v>40882</v>
       </c>
-      <c r="M19" s="29"/>
-      <c r="N19" s="20"/>
-      <c r="O19" s="20"/>
-      <c r="P19" s="21"/>
+      <c r="M19" s="18"/>
+      <c r="N19" s="19"/>
+      <c r="O19" s="19"/>
+      <c r="P19" s="20"/>
       <c r="Q19" s="12"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
@@ -1627,10 +1598,10 @@
       <c r="L20" s="14">
         <v>40889</v>
       </c>
-      <c r="M20" s="29"/>
-      <c r="N20" s="20"/>
-      <c r="O20" s="20"/>
-      <c r="P20" s="21"/>
+      <c r="M20" s="18"/>
+      <c r="N20" s="19"/>
+      <c r="O20" s="19"/>
+      <c r="P20" s="20"/>
       <c r="Q20" s="16" t="s">
         <v>49</v>
       </c>
@@ -1663,7 +1634,7 @@
       <c r="L21" s="15">
         <v>40896</v>
       </c>
-      <c r="M21" s="30"/>
+      <c r="M21" s="21"/>
       <c r="N21" s="22"/>
       <c r="O21" s="22"/>
       <c r="P21" s="23"/>
@@ -1828,7 +1799,7 @@
         <v>56</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
@@ -1848,7 +1819,7 @@
         <v>56</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
@@ -1931,8 +1902,59 @@
         <v>16</v>
       </c>
     </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>30</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>31</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="L3:Q3"/>
+    <mergeCell ref="L4:Q4"/>
+    <mergeCell ref="L5:Q5"/>
+    <mergeCell ref="I8:Q8"/>
+    <mergeCell ref="I2:Q2"/>
+    <mergeCell ref="M9:P9"/>
+    <mergeCell ref="M10:P10"/>
+    <mergeCell ref="M11:P11"/>
+    <mergeCell ref="M12:P12"/>
+    <mergeCell ref="M13:P13"/>
     <mergeCell ref="M20:P20"/>
     <mergeCell ref="M21:P21"/>
     <mergeCell ref="M14:P14"/>
@@ -1941,31 +1963,20 @@
     <mergeCell ref="M17:P17"/>
     <mergeCell ref="M18:P18"/>
     <mergeCell ref="M19:P19"/>
-    <mergeCell ref="M9:P9"/>
-    <mergeCell ref="M10:P10"/>
-    <mergeCell ref="M11:P11"/>
-    <mergeCell ref="M12:P12"/>
-    <mergeCell ref="M13:P13"/>
-    <mergeCell ref="L3:Q3"/>
-    <mergeCell ref="L4:Q4"/>
-    <mergeCell ref="L5:Q5"/>
-    <mergeCell ref="I8:Q8"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="I2:Q2"/>
   </mergeCells>
-  <conditionalFormatting sqref="F4:F34">
-    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="NOT STARTED">
+  <conditionalFormatting sqref="F4:F36">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="NOT STARTED">
       <formula>NOT(ISERROR(SEARCH("NOT STARTED",F4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="IN PROGRESS">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="IN PROGRESS">
       <formula>NOT(ISERROR(SEARCH("IN PROGRESS",F4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",F4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F34">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F36">
       <formula1>$I$3:$I$5</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>